<commit_message>
Final changes before hand-in.
</commit_message>
<xml_diff>
--- a/data/samples-intensities.xlsx
+++ b/data/samples-intensities.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFB85221-97C5-47B3-AD08-87A499380A3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053F786B-3589-4A09-8DBF-010C46BD1928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22680" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="semicon" sheetId="1" r:id="rId1"/>
     <sheet name="alloys" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -486,15 +495,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -521,8 +530,12 @@
       <c r="D2">
         <v>122.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>D2/20</f>
+        <v>6.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -535,8 +548,12 @@
       <c r="D3">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="0">D3/20</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -549,8 +566,12 @@
       <c r="D4" s="2">
         <v>42.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>2.1399999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -563,8 +584,12 @@
       <c r="D5">
         <v>266.11</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>13.3055</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -576,6 +601,19 @@
       </c>
       <c r="D6">
         <v>38.4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2.86</v>
+      </c>
+      <c r="C8">
+        <f>B8*SQRT(2)/20</f>
+        <v>0.20223253941935257</v>
       </c>
     </row>
   </sheetData>
@@ -585,20 +623,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA45797-EC6A-4906-AED0-F0810CC2E582}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H28"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="4" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="7" width="17.140625" customWidth="1"/>
+    <col min="12" max="13" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,23 +649,28 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="3"/>
+      <c r="P1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -641,29 +684,49 @@
         <v>381.9</v>
       </c>
       <c r="E2">
+        <f>D2/20</f>
+        <v>19.094999999999999</v>
+      </c>
+      <c r="F2">
         <f>D2/D3</f>
         <v>5.5508720930232558</v>
       </c>
-      <c r="F2">
+      <c r="G2">
+        <f>F2*SQRT(2)/20</f>
+        <v>0.39250592984759086</v>
+      </c>
+      <c r="H2">
         <f>D2/D4</f>
         <v>0.42287675783412687</v>
       </c>
-      <c r="G2">
-        <f>F2/(1+F2)</f>
+      <c r="I2">
+        <f>H2*SQRT(2)/20</f>
+        <v>2.990190230706926E-2</v>
+      </c>
+      <c r="J2">
+        <f>H2/(1+H2)</f>
         <v>0.29719844357976655</v>
       </c>
-      <c r="H2">
-        <f>(G2*$K$2)/(G2*$K$2 + G4*$K$3)</f>
+      <c r="K2">
+        <f>J2/10</f>
+        <v>2.9719844357976654E-2</v>
+      </c>
+      <c r="L2">
+        <f>(J2*$P$2)/(J2*$P$2 + J4*$P$3)</f>
         <v>0.27755539703162702</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2">
+        <f>L2/10</f>
+        <v>2.7755539703162701E-2</v>
+      </c>
+      <c r="O2" t="s">
         <v>28</v>
       </c>
-      <c r="K2">
+      <c r="P2">
         <v>7.15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -676,14 +739,34 @@
       <c r="D3">
         <v>68.8</v>
       </c>
-      <c r="J3" t="s">
+      <c r="E3">
+        <f t="shared" ref="E3:E28" si="0">D3/20</f>
+        <v>3.44</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G28" si="1">F3*SQRT(2)/20</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I28" si="2">H3*SQRT(2)/20</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K28" si="3">J3/10</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M28" si="4">L3/10</f>
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
         <v>29</v>
       </c>
-      <c r="K3">
+      <c r="P3">
         <v>7.87</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -697,25 +780,45 @@
         <v>903.1</v>
       </c>
       <c r="E4">
+        <f t="shared" si="0"/>
+        <v>45.155000000000001</v>
+      </c>
+      <c r="F4">
         <f>D4/D5</f>
         <v>4.1388634280476628</v>
       </c>
       <c r="G4">
-        <f>1/(1+F2)</f>
+        <f t="shared" si="1"/>
+        <v>0.29266183963775028</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>1/(1+H2)</f>
         <v>0.70280155642023345</v>
       </c>
-      <c r="H4">
-        <f>1-H2</f>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>7.0280155642023348E-2</v>
+      </c>
+      <c r="L4">
+        <f>1-L2</f>
         <v>0.72244460296837298</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4">
+        <f t="shared" si="4"/>
+        <v>7.2244460296837301E-2</v>
+      </c>
+      <c r="O4" t="s">
         <v>30</v>
       </c>
-      <c r="K4">
+      <c r="P4">
         <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -728,18 +831,38 @@
       <c r="D5" s="2">
         <v>218.2</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>10.91</v>
+      </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H5" s="2"/>
-      <c r="J5" t="s">
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
         <v>31</v>
       </c>
-      <c r="K5">
+      <c r="P5">
         <v>7.1340000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -753,23 +876,43 @@
         <v>2110.1999999999998</v>
       </c>
       <c r="E6">
+        <f t="shared" si="0"/>
+        <v>105.50999999999999</v>
+      </c>
+      <c r="F6">
         <f>D6/D7</f>
         <v>6.1360860715324224</v>
       </c>
-      <c r="F6">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.43388680711248984</v>
+      </c>
+      <c r="H6">
         <f>D6/D8</f>
         <v>1.783920872432158</v>
       </c>
-      <c r="G6">
-        <f>F6/(1+F6)</f>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>0.1261422545997001</v>
+      </c>
+      <c r="J6">
+        <f>H6/(1+H6)</f>
         <v>0.64079438826637514</v>
       </c>
-      <c r="H6">
-        <f>(G6*$K$4)/(G6*$K$4 + G8*$K$5)</f>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>6.4079438826637511E-2</v>
+      </c>
+      <c r="L6">
+        <f>(J6*$P$4)/(J6*$P$4 + J8*$P$5)</f>
         <v>0.69140837063851579</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>6.9140837063851573E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -782,8 +925,28 @@
       <c r="D7" s="3">
         <v>343.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>17.195</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -797,19 +960,39 @@
         <v>1182.9000000000001</v>
       </c>
       <c r="E8">
+        <f t="shared" si="0"/>
+        <v>59.145000000000003</v>
+      </c>
+      <c r="F8">
         <f>D8/D9</f>
         <v>17.093930635838152</v>
       </c>
       <c r="G8">
-        <f>1/(1+F6)</f>
+        <f t="shared" si="1"/>
+        <v>1.2087234269733629</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f>1/(1+H6)</f>
         <v>0.35920561173362492</v>
       </c>
-      <c r="H8">
-        <f>1-H6</f>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>3.5920561173362495E-2</v>
+      </c>
+      <c r="L8">
+        <f>1-L6</f>
         <v>0.30859162936148421</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>3.0859162936148422E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -822,12 +1005,32 @@
       <c r="D9" s="4">
         <v>69.2</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3.46</v>
+      </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -841,23 +1044,43 @@
         <v>3947.9</v>
       </c>
       <c r="E10">
+        <f t="shared" si="0"/>
+        <v>197.39500000000001</v>
+      </c>
+      <c r="F10">
         <f>D10/D11</f>
         <v>14.329945553539019</v>
       </c>
-      <c r="F10">
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1.0132801674941456</v>
+      </c>
+      <c r="H10">
         <f>D10/D12</f>
         <v>1.2655148095909732</v>
       </c>
-      <c r="G10">
-        <f>F10/(1+F10)</f>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>8.9485410355377965E-2</v>
+      </c>
+      <c r="J10">
+        <f>H10/(1+H10)</f>
         <v>0.55859922178988319</v>
       </c>
-      <c r="H10">
-        <f>(G10*$K$4)/(G10*$K$4 + G12*$K$5)</f>
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>5.5859922178988317E-2</v>
+      </c>
+      <c r="L10">
+        <f>(J10*$P$4)/(J10*$P$4 + J12*$P$5)</f>
         <v>0.61381502204336358</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>6.1381502204336358E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -870,8 +1093,28 @@
       <c r="D11" s="3">
         <v>275.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>13.775</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -885,19 +1128,39 @@
         <v>3119.6</v>
       </c>
       <c r="E12">
+        <f t="shared" si="0"/>
+        <v>155.97999999999999</v>
+      </c>
+      <c r="F12">
         <f>D12/D13</f>
         <v>16.514557967178401</v>
       </c>
       <c r="G12">
-        <f>1/(1+F10)</f>
+        <f t="shared" si="1"/>
+        <v>1.1677555926890173</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f>1/(1+H10)</f>
         <v>0.4414007782101167</v>
       </c>
-      <c r="H12">
-        <f>1-H10</f>
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>4.4140077821011668E-2</v>
+      </c>
+      <c r="L12">
+        <f>1-L10</f>
         <v>0.38618497795663642</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>3.8618497795663641E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -910,12 +1173,32 @@
       <c r="D13" s="2">
         <v>188.9</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>9.4450000000000003</v>
+      </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
@@ -924,12 +1207,32 @@
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="6"/>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -938,12 +1241,32 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
@@ -957,23 +1280,43 @@
         <v>1351.9</v>
       </c>
       <c r="E16">
+        <f t="shared" si="0"/>
+        <v>67.594999999999999</v>
+      </c>
+      <c r="F16">
         <f>D16/D17</f>
         <v>3.7365948037589831</v>
       </c>
-      <c r="F16">
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>0.26421715242843941</v>
+      </c>
+      <c r="H16">
         <f>D16/D18</f>
         <v>2.0620805369127519</v>
       </c>
-      <c r="G16">
-        <f>F16/(1+F16)</f>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>0.14581111310038036</v>
+      </c>
+      <c r="J16">
+        <f>H16/(1+H16)</f>
         <v>0.67342465753424663</v>
       </c>
-      <c r="H16">
-        <f>(G16*$K$3)/(G16*$K$3 + G18*$K$5)</f>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>6.734246575342466E-2</v>
+      </c>
+      <c r="L16">
+        <f>(J16*$P$3)/(J16*$P$3 + J18*$P$5)</f>
         <v>0.69463980924001234</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>6.9463980924001231E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -986,11 +1329,31 @@
       <c r="D17" s="3">
         <v>361.8</v>
       </c>
-      <c r="E17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>18.09</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17"/>
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L17"/>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -1004,19 +1367,39 @@
         <v>655.6</v>
       </c>
       <c r="E18">
+        <f t="shared" si="0"/>
+        <v>32.78</v>
+      </c>
+      <c r="F18">
         <f>D18/D19</f>
         <v>8.5699346405228756</v>
       </c>
       <c r="G18">
-        <f>1/(1+F16)</f>
+        <f t="shared" si="1"/>
+        <v>0.60598588986392232</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>1/(1+H16)</f>
         <v>0.32657534246575337</v>
       </c>
-      <c r="H18">
-        <f>1-H16</f>
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>3.2657534246575338E-2</v>
+      </c>
+      <c r="L18">
+        <f>1-L16</f>
         <v>0.30536019075998766</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <f t="shared" si="4"/>
+        <v>3.0536019075998767E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -1029,12 +1412,32 @@
       <c r="D19" s="4">
         <v>76.5</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>3.8250000000000002</v>
+      </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1048,23 +1451,43 @@
         <v>1443.6</v>
       </c>
       <c r="E20">
+        <f t="shared" si="0"/>
+        <v>72.179999999999993</v>
+      </c>
+      <c r="F20">
         <f>D20/D21</f>
         <v>3.9217603911980436</v>
       </c>
-      <c r="F20">
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>0.27731033668049443</v>
+      </c>
+      <c r="H20">
         <f>D20/D22</f>
         <v>3.4216639013984356</v>
       </c>
-      <c r="G20">
-        <f>F20/(1+F20)</f>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>0.24194817476200522</v>
+      </c>
+      <c r="J20">
+        <f>H20/(1+H20)</f>
         <v>0.7738407933529885</v>
       </c>
-      <c r="H20">
-        <f>(G20*$K$3)/(G20*$K$3 + G22*$K$5)</f>
+      <c r="K20">
+        <f t="shared" si="3"/>
+        <v>7.7384079335298853E-2</v>
+      </c>
+      <c r="L20">
+        <f>(J20*$P$3)/(J20*$P$3 + J22*$P$5)</f>
         <v>0.79056143655639688</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <f t="shared" si="4"/>
+        <v>7.9056143655639691E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -1077,8 +1500,28 @@
       <c r="D21" s="3">
         <v>368.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>18.405000000000001</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1092,19 +1535,39 @@
         <v>421.9</v>
       </c>
       <c r="E22">
+        <f t="shared" si="0"/>
+        <v>21.094999999999999</v>
+      </c>
+      <c r="F22">
         <f>D22/D23</f>
         <v>9.74364896073903</v>
       </c>
       <c r="G22">
-        <f>1/(1+F20)</f>
+        <f t="shared" si="1"/>
+        <v>0.68898002536398251</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f>1/(1+H20)</f>
         <v>0.22615920664701153</v>
       </c>
-      <c r="H22">
-        <f>1-H20</f>
+      <c r="K22">
+        <f t="shared" si="3"/>
+        <v>2.2615920664701153E-2</v>
+      </c>
+      <c r="L22">
+        <f>1-L20</f>
         <v>0.20943856344360312</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <f t="shared" si="4"/>
+        <v>2.0943856344360311E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -1117,12 +1580,32 @@
       <c r="D23" s="4">
         <v>43.3</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>2.165</v>
+      </c>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1131,12 +1614,32 @@
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="6"/>
+      <c r="K24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="6"/>
+      <c r="M24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -1150,23 +1653,43 @@
         <v>1443.3</v>
       </c>
       <c r="E25">
+        <f t="shared" si="0"/>
+        <v>72.164999999999992</v>
+      </c>
+      <c r="F25">
         <f>D25/D26</f>
         <v>3.8850605652759085</v>
       </c>
-      <c r="F25">
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>0.27471526710270366</v>
+      </c>
+      <c r="H25">
         <f>D25/D27</f>
         <v>2.5594963646036533</v>
       </c>
-      <c r="G25">
-        <f>F25/(1+F25)</f>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>0.18098372358335596</v>
+      </c>
+      <c r="J25">
+        <f>H25/(1+H25)</f>
         <v>0.71906137903547229</v>
       </c>
-      <c r="H25">
-        <f>(G25*$K$3)/(G25*$K$3 + G27*$K$5)</f>
+      <c r="K25">
+        <f t="shared" si="3"/>
+        <v>7.1906137903547232E-2</v>
+      </c>
+      <c r="L25">
+        <f>(J25*$P$3)/(J25*$P$3 + J27*$P$5)</f>
         <v>0.73846324099151606</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <f t="shared" si="4"/>
+        <v>7.3846324099151608E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
@@ -1179,8 +1702,28 @@
       <c r="D26" s="3">
         <v>371.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>18.574999999999999</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
@@ -1194,19 +1737,39 @@
         <v>563.9</v>
       </c>
       <c r="E27">
+        <f t="shared" si="0"/>
+        <v>28.195</v>
+      </c>
+      <c r="F27">
         <f>D27/D28</f>
         <v>9.367109634551495</v>
       </c>
       <c r="G27">
-        <f>1/(1+F25)</f>
+        <f t="shared" si="1"/>
+        <v>0.66235467427092054</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f>1/(1+H25)</f>
         <v>0.28093862096452771</v>
       </c>
-      <c r="H27">
-        <f>1-H25</f>
+      <c r="K27">
+        <f t="shared" si="3"/>
+        <v>2.809386209645277E-2</v>
+      </c>
+      <c r="L27">
+        <f>1-L25</f>
         <v>0.26153675900848394</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <f t="shared" si="4"/>
+        <v>2.6153675900848394E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
@@ -1219,10 +1782,35 @@
       <c r="D28" s="4">
         <v>60.2</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>3.0100000000000002</v>
+      </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H28" s="2"/>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>122.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>